<commit_message>
Make models, validation results, and plots for publication.
</commit_message>
<xml_diff>
--- a/2016-06-22/validation_props.xlsx
+++ b/2016-06-22/validation_props.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26230"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinyang/Documents/Projects/Twist_Project/2016-06-22/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15000" tabRatio="500"/>
   </bookViews>
@@ -51,9 +56,6 @@
     <t>pix_ratio_std</t>
   </si>
   <si>
-    <t>intensity_ratio_mean</t>
-  </si>
-  <si>
     <t>intensity_ratio_std</t>
   </si>
   <si>
@@ -103,6 +105,9 @@
   </si>
   <si>
     <t>c4_2</t>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
   </si>
 </sst>
 </file>
@@ -146,6 +151,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -474,14 +484,14 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -514,18 +524,18 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -567,9 +577,9 @@
         <v>1.00085726924</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>0.77367895787600005</v>
@@ -611,9 +621,9 @@
         <v>0.37807644767300003</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>0.79380232787399996</v>
@@ -655,9 +665,9 @@
         <v>0.39152993634299998</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>0.108467301712</v>
@@ -699,9 +709,9 @@
         <v>6.9983571717300002E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>0.189803440293</v>
@@ -743,9 +753,9 @@
         <v>8.0518984906300002E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>9.0223118821300005E-2</v>
@@ -787,9 +797,9 @@
         <v>3.9906494710999999E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>0.58284288552200003</v>
@@ -831,9 +841,9 @@
         <v>0.17254108608900001</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>0.864578637293</v>
@@ -875,9 +885,9 @@
         <v>0.53822437782200006</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>0.24863667381900001</v>
@@ -919,9 +929,9 @@
         <v>9.2778260371E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>0.167172274165</v>
@@ -963,9 +973,9 @@
         <v>5.9276266146500002E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>0.86807082513300005</v>
@@ -1007,9 +1017,9 @@
         <v>0.92380183195900001</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>1.0010455476</v>
@@ -1051,9 +1061,9 @@
         <v>0.70319348315800001</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14">
         <v>0.17877448773599999</v>
@@ -1095,9 +1105,9 @@
         <v>5.2199223956099997E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15">
         <v>1.0412877525599999</v>
@@ -1141,10 +1151,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>